<commit_message>
Wrote Carpals-Metacarpals Kinematics Transform Data to File
- Added Transform Measurement Blocks for Carpals-Metacarpals Joints
- Wrote Carpals-Metacarpals Kinematics Transform Data to File
</commit_message>
<xml_diff>
--- a/Analysis and Results/Digits Kinematics Data.xlsx
+++ b/Analysis and Results/Digits Kinematics Data.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="91">
   <si>
     <t>DP_Length</t>
   </si>
@@ -169,6 +169,123 @@
   </si>
   <si>
     <t>MC_head_ligament_length</t>
+  </si>
+  <si>
+    <t>DP_Length</t>
+  </si>
+  <si>
+    <t>MP_Length</t>
+  </si>
+  <si>
+    <t>PP_Length</t>
+  </si>
+  <si>
+    <t>MC_Lenght</t>
+  </si>
+  <si>
+    <t>IP_Joint_Radius</t>
+  </si>
+  <si>
+    <t>DIP_Joint_Radius</t>
+  </si>
+  <si>
+    <t>PIP_Joint_Radius</t>
+  </si>
+  <si>
+    <t>MCP_Joint_Radius</t>
+  </si>
+  <si>
+    <t>IP_Joint_Length</t>
+  </si>
+  <si>
+    <t>DIP_Joint_Length</t>
+  </si>
+  <si>
+    <t>PIP_Joint_Length</t>
+  </si>
+  <si>
+    <t>MCP_Joint_Length</t>
+  </si>
+  <si>
+    <t>MC_head_ligament_length</t>
+  </si>
+  <si>
+    <t>DP_Length (m)</t>
+  </si>
+  <si>
+    <t>MP_Length (m)</t>
+  </si>
+  <si>
+    <t>PP_Length (m)</t>
+  </si>
+  <si>
+    <t>MC_Lenght (m)</t>
+  </si>
+  <si>
+    <t>IP_Joint_Radius (m)</t>
+  </si>
+  <si>
+    <t>DIP_Joint_Radius (m)</t>
+  </si>
+  <si>
+    <t>PIP_Joint_Radius (m)</t>
+  </si>
+  <si>
+    <t>MCP_Joint_Radius (m)</t>
+  </si>
+  <si>
+    <t>IP_Joint_Length (m)</t>
+  </si>
+  <si>
+    <t>DIP_Joint_Length (m)</t>
+  </si>
+  <si>
+    <t>PIP_Joint_Length (m)</t>
+  </si>
+  <si>
+    <t>MCP_Joint_Length (m)</t>
+  </si>
+  <si>
+    <t>MC_head_ligament_length (m)</t>
+  </si>
+  <si>
+    <t>DP_Length (m)</t>
+  </si>
+  <si>
+    <t>MP_Length (m)</t>
+  </si>
+  <si>
+    <t>PP_Length (m)</t>
+  </si>
+  <si>
+    <t>MC_Lenght (m)</t>
+  </si>
+  <si>
+    <t>IP_Joint_Radius (m)</t>
+  </si>
+  <si>
+    <t>DIP_Joint_Radius (m)</t>
+  </si>
+  <si>
+    <t>PIP_Joint_Radius (m)</t>
+  </si>
+  <si>
+    <t>MCP_Joint_Radius (m)</t>
+  </si>
+  <si>
+    <t>IP_Joint_Length (m)</t>
+  </si>
+  <si>
+    <t>DIP_Joint_Length (m)</t>
+  </si>
+  <si>
+    <t>PIP_Joint_Length (m)</t>
+  </si>
+  <si>
+    <t>MCP_Joint_Length (m)</t>
+  </si>
+  <si>
+    <t>MC_head_ligament_length (m)</t>
   </si>
 </sst>
 </file>
@@ -189,7 +306,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -201,16 +318,22 @@
     <border/>
     <border/>
     <border/>
+    <border/>
+    <border/>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -224,59 +347,59 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="14.7109375" customWidth="true"/>
-    <col min="2" max="2" width="13.7109375" customWidth="true"/>
-    <col min="3" max="3" width="13.7109375" customWidth="true"/>
-    <col min="4" max="4" width="13.7109375" customWidth="true"/>
-    <col min="5" max="5" width="15" customWidth="true"/>
-    <col min="6" max="6" width="16.28515625" customWidth="true"/>
-    <col min="7" max="7" width="16.140625" customWidth="true"/>
-    <col min="8" max="8" width="17.28515625" customWidth="true"/>
-    <col min="9" max="9" width="15.140625" customWidth="true"/>
-    <col min="10" max="10" width="16.42578125" customWidth="true"/>
-    <col min="11" max="11" width="16.28515625" customWidth="true"/>
-    <col min="12" max="12" width="17.42578125" customWidth="true"/>
-    <col min="13" max="13" width="25" customWidth="true"/>
+    <col min="2" max="2" width="14.5703125" customWidth="true"/>
+    <col min="3" max="3" width="14" customWidth="true"/>
+    <col min="4" max="4" width="14.5703125" customWidth="true"/>
+    <col min="5" max="5" width="18.5703125" customWidth="true"/>
+    <col min="6" max="6" width="19.85546875" customWidth="true"/>
+    <col min="7" max="7" width="19.7109375" customWidth="true"/>
+    <col min="8" max="8" width="20.85546875" customWidth="true"/>
+    <col min="9" max="9" width="18.7109375" customWidth="true"/>
+    <col min="10" max="10" width="20" customWidth="true"/>
+    <col min="11" max="11" width="19.85546875" customWidth="true"/>
+    <col min="12" max="12" width="21" customWidth="true"/>
+    <col min="13" max="13" width="28.5703125" customWidth="true"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="0" t="s">
-        <v>39</v>
+        <v>78</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>40</v>
+        <v>79</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>41</v>
+        <v>80</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>42</v>
+        <v>81</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>43</v>
+        <v>82</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>44</v>
+        <v>83</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>45</v>
+        <v>84</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>46</v>
+        <v>85</v>
       </c>
       <c r="I1" s="0" t="s">
-        <v>47</v>
+        <v>86</v>
       </c>
       <c r="J1" s="0" t="s">
-        <v>48</v>
+        <v>87</v>
       </c>
       <c r="K1" s="0" t="s">
-        <v>49</v>
+        <v>88</v>
       </c>
       <c r="L1" s="0" t="s">
-        <v>50</v>
+        <v>89</v>
       </c>
       <c r="M1" s="0" t="s">
-        <v>51</v>
+        <v>90</v>
       </c>
     </row>
     <row r="2">

</xml_diff>